<commit_message>
New tag definitions. Updated template. Enhancements for duplicate headers.
</commit_message>
<xml_diff>
--- a/public/test/metadata_template.xlsx
+++ b/public/test/metadata_template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>filename</t>
   </si>
@@ -25,18 +25,21 @@
     <t>identifier-IID</t>
   </si>
   <si>
-    <t>title-nonsort</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
+    <t>Title-nonsort</t>
+  </si>
+  <si>
     <t>title-alternative</t>
   </si>
   <si>
     <t>name-personal-primary</t>
   </si>
   <si>
+    <t>role</t>
+  </si>
+  <si>
     <t>name-personal-primary-date</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t>name-personal-date</t>
   </si>
   <si>
+    <t>name-corporate</t>
+  </si>
+  <si>
     <t>type of resource</t>
   </si>
   <si>
@@ -61,19 +67,22 @@
     <t>date created</t>
   </si>
   <si>
+    <t>date issued</t>
+  </si>
+  <si>
     <t>issuance</t>
   </si>
   <si>
-    <t>physical-form</t>
-  </si>
-  <si>
     <t>language</t>
   </si>
   <si>
     <t>iso-lang</t>
   </si>
   <si>
-    <t>description</t>
+    <t>physicalDescription</t>
+  </si>
+  <si>
+    <t>physicalDescription-extent</t>
   </si>
   <si>
     <t>access condition</t>
@@ -85,18 +94,46 @@
     <t>subject-topic-lcsh</t>
   </si>
   <si>
+    <t>subject-title</t>
+  </si>
+  <si>
     <t>subject-geographic</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>note type</t>
+  </si>
+  <si>
+    <t>related item title</t>
+  </si>
+  <si>
+    <t>table of contents</t>
+  </si>
+  <si>
+    <t>provenance</t>
+  </si>
+  <si>
+    <t>location URL</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
+    <numFmt formatCode="@" numFmtId="166"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -133,6 +170,13 @@
       <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="5">
@@ -195,7 +239,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -204,7 +248,31 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="5" numFmtId="166" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="4" numFmtId="166" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -212,27 +280,11 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -313,42 +365,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X65536"/>
+  <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2:X2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="I1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="L9" activeCellId="0" pane="topLeft" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.004048582996"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.8502024291498"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.9959514170041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="31.5708502024291"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="37.8542510121458"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="41.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="27.5708502024291"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.21862348178138"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.2793522267206"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.21862348178138"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="23.8178137651822"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="23.5748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="31.5708502024291"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="18.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="30.8582995951417"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="20.004048582996"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="25"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="26.1457489878542"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.1457489878542"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="23.4251012145749"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="30.7125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.74089068825911"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.5708502024291"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.5748987854251"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="31.5708502024291"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="19.5748987854251"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="18.1376518218623"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="30.8582995951417"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="17.4251012145749"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="20.004048582996"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="27.1457489878542"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="32.7125506072874"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="25"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="26.1457489878542"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="23.1457489878542"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="23.4251012145749"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="24"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="12.7125506072875"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="22.4251012145749"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="23.8502024291498"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1023" min="38" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="18.75" outlineLevel="0" r="1" s="3">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="17.9" outlineLevel="0" r="1" s="9">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -370,214 +436,108 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="R1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="S1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="Z1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048423"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048424"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048425"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048426"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048427"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048428"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048429"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048430"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048431"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048432"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048433"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048434"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048435"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048436"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048437"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048438"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048439"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048440"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048441"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048442"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048443"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048444"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048445"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048446"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048447"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048448"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048449"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048450"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048451"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048452"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048453"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048454"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048455"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048456"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048457"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048458"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048459"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048460"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048461"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048462"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048463"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048464"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048465"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048466"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048467"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048468"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048469"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048470"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048471"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048472"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048473"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048474"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048475"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048476"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048477"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048478"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048479"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048480"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048481"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048482"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048483"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048484"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048485"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048486"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048487"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048488"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048489"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048490"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048491"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048492"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048493"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048494"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048495"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048496"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048497"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048498"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048499"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048500"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048501"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048502"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048503"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048504"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048505"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048506"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048507"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048508"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048509"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048510"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048511"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048512"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048513"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048514"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048515"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048516"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048517"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048518"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048519"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048520"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048521"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048522"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048523"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048524"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048525"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048526"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048527"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048528"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048529"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048530"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048531"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048532"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048533"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048534"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048535"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048536"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048537"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048538"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048539"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048540"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048541"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048542"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048543"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048544"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048545"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048546"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048547"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048548"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048549"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048550"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048551"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048552"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048553"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048554"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048555"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048556"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048557"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048558"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048559"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048560"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048561"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048562"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048563"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048564"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048565"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048566"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048567"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048568"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048569"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048570"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048571"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048572"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048573"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048574"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048575"/>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
+      <c r="A3" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -597,12 +557,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A2:X2 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -623,12 +583,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A2:X2 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>